<commit_message>
add T4.4a Semi-arid woodlands
</commit_message>
<xml_diff>
--- a/IUCNGET_Classes.xlsx
+++ b/IUCNGET_Classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EC09FCF-6589-4FDF-B0FD-C332436218ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB642E0-1422-46F0-B40D-39A26080270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9592630E-38D2-4D1A-AB21-F40B7D1DFF27}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9592630E-38D2-4D1A-AB21-F40B7D1DFF27}"/>
   </bookViews>
   <sheets>
     <sheet name="Final list" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="322">
   <si>
     <t>Realm</t>
   </si>
@@ -1000,13 +1000,22 @@
   </si>
   <si>
     <t>TF1.1</t>
+  </si>
+  <si>
+    <t>Semi-arid woodlands</t>
+  </si>
+  <si>
+    <t>T4.4a</t>
+  </si>
+  <si>
+    <t>Extra class from IUCNGET added by D. Keith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1049,6 +1058,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1076,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1096,6 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1430,27 +1446,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F06308A-2E28-46FE-9E09-C3F62953F32E}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="77.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="77.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
@@ -1485,7 +1501,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1521,7 +1537,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1557,7 +1573,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1593,7 +1609,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1629,7 +1645,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1665,7 +1681,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1701,7 +1717,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1731,7 +1747,7 @@
       </c>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1767,7 +1783,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1803,7 +1819,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1839,7 +1855,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1874,7 +1890,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1910,7 +1926,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1946,7 +1962,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1982,7 +1998,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2018,7 +2034,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2048,7 +2064,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2078,7 +2094,7 @@
       </c>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2112,7 +2128,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2146,7 +2162,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2180,7 +2196,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2214,7 +2230,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2248,7 +2264,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2278,7 +2294,7 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2314,7 +2330,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2350,7 +2366,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2380,7 +2396,7 @@
       </c>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2414,7 +2430,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2448,7 +2464,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2484,7 +2500,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2518,7 +2534,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2554,7 +2570,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2587,7 +2603,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2621,7 +2637,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2651,7 +2667,7 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2684,7 +2700,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2717,7 +2733,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2750,7 +2766,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2783,7 +2799,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2812,7 +2828,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2841,7 +2857,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2870,7 +2886,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2903,7 +2919,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2936,7 +2952,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2969,7 +2985,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3002,7 +3018,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3035,7 +3051,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3068,7 +3084,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3097,7 +3113,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3126,7 +3142,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3155,7 +3171,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3188,7 +3204,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3221,7 +3237,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3254,7 +3270,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3287,7 +3303,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3320,7 +3336,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3349,7 +3365,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3382,7 +3398,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3411,7 +3427,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3440,7 +3456,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3469,7 +3485,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3498,7 +3514,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3531,7 +3547,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3564,7 +3580,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3593,7 +3609,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3626,7 +3642,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3659,7 +3675,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3692,7 +3708,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3725,7 +3741,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3758,7 +3774,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3787,7 +3803,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3820,7 +3836,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3853,7 +3869,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3886,7 +3902,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3919,7 +3935,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3952,7 +3968,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3981,7 +3997,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4015,7 +4031,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>79</v>
       </c>
@@ -4048,7 +4064,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>80</v>
       </c>
@@ -4081,7 +4097,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>81</v>
       </c>
@@ -4114,7 +4130,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>82</v>
       </c>
@@ -4147,7 +4163,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>83</v>
       </c>
@@ -4180,7 +4196,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>84</v>
       </c>
@@ -4213,7 +4229,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>85</v>
       </c>
@@ -4246,7 +4262,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>86</v>
       </c>
@@ -4276,7 +4292,7 @@
       </c>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>78</v>
       </c>
@@ -4309,12 +4325,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" ref="B88:B101" si="2">CONCATENATE(H88," ",G88)</f>
+        <f t="shared" ref="B88:B102" si="2">CONCATENATE(H88," ",G88)</f>
         <v>M2.1 Epipelagic ocean waters</v>
       </c>
       <c r="C88" t="s">
@@ -4342,7 +4358,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4375,7 +4391,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4408,7 +4424,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4441,7 +4457,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4471,7 +4487,7 @@
       </c>
       <c r="K92" s="7"/>
     </row>
-    <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4504,7 +4520,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4537,7 +4553,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4570,7 +4586,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4603,7 +4619,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4633,7 +4649,7 @@
       </c>
       <c r="K97" s="7"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4663,7 +4679,7 @@
       </c>
       <c r="K98" s="7"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4693,7 +4709,7 @@
       </c>
       <c r="K99" s="7"/>
     </row>
-    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4729,7 +4745,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4763,6 +4779,42 @@
       </c>
       <c r="K101" s="7" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="str">
+        <f t="shared" si="2"/>
+        <v>T4.4a Semi-arid woodlands</v>
+      </c>
+      <c r="C102" t="s">
+        <v>86</v>
+      </c>
+      <c r="D102" t="s">
+        <v>87</v>
+      </c>
+      <c r="E102" t="s">
+        <v>112</v>
+      </c>
+      <c r="F102" t="s">
+        <v>113</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H102" t="s">
+        <v>320</v>
+      </c>
+      <c r="I102" t="s">
+        <v>241</v>
+      </c>
+      <c r="J102" t="s">
+        <v>321</v>
+      </c>
+      <c r="K102" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -5010,15 +5062,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="44e1a4a7-75d8-43f0-81dc-4aceded6063f">
@@ -5047,6 +5090,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99AD8296-EEAC-435D-8285-7496ACD2EECA}">
   <ds:schemaRefs>
@@ -5067,14 +5119,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E49A9ABC-A427-42A2-8F7A-D6C6654B9600}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36EA50D7-0A13-4ECA-8436-D4585B901078}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -5089,4 +5133,12 @@
     <ds:schemaRef ds:uri="27145d01-5063-4320-a0f8-74c9d44fede6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E49A9ABC-A427-42A2-8F7A-D6C6654B9600}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add unclassified as 255
</commit_message>
<xml_diff>
--- a/IUCNGET_Classes.xlsx
+++ b/IUCNGET_Classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB642E0-1422-46F0-B40D-39A26080270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31BC18A-3C28-469A-AFB5-944A9E6DF301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9592630E-38D2-4D1A-AB21-F40B7D1DFF27}"/>
+    <workbookView xWindow="-25710" yWindow="7090" windowWidth="25820" windowHeight="13900" xr2:uid="{9592630E-38D2-4D1A-AB21-F40B7D1DFF27}"/>
   </bookViews>
   <sheets>
     <sheet name="Final list" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="323">
   <si>
     <t>Realm</t>
   </si>
@@ -1009,6 +1009,9 @@
   </si>
   <si>
     <t>Extra class from IUCNGET added by D. Keith</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
   </si>
 </sst>
 </file>
@@ -1446,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F06308A-2E28-46FE-9E09-C3F62953F32E}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="G115" sqref="G115"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4815,6 +4818,18 @@
       </c>
       <c r="K102" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>255</v>
+      </c>
+      <c r="B103" t="str">
+        <f t="shared" ref="B103" si="3">CONCATENATE(H103," ",G103)</f>
+        <v xml:space="preserve"> Unclassified</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -5062,6 +5077,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="44e1a4a7-75d8-43f0-81dc-4aceded6063f">
@@ -5090,15 +5114,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99AD8296-EEAC-435D-8285-7496ACD2EECA}">
   <ds:schemaRefs>
@@ -5119,6 +5134,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E49A9ABC-A427-42A2-8F7A-D6C6654B9600}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36EA50D7-0A13-4ECA-8436-D4585B901078}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -5133,12 +5156,4 @@
     <ds:schemaRef ds:uri="27145d01-5063-4320-a0f8-74c9d44fede6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E49A9ABC-A427-42A2-8F7A-D6C6654B9600}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
revise the column names
</commit_message>
<xml_diff>
--- a/IUCNGET_Classes.xlsx
+++ b/IUCNGET_Classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31BC18A-3C28-469A-AFB5-944A9E6DF301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F676BE-0808-4DB0-8F51-2CC722CC8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="7090" windowWidth="25820" windowHeight="13900" xr2:uid="{9592630E-38D2-4D1A-AB21-F40B7D1DFF27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="323">
   <si>
     <t>Realm</t>
   </si>
@@ -674,9 +674,6 @@
     <t>UID</t>
   </si>
   <si>
-    <t>object_label</t>
-  </si>
-  <si>
     <t>OzEstuaries100K</t>
   </si>
   <si>
@@ -684,9 +681,6 @@
   </si>
   <si>
     <t>Data source</t>
-  </si>
-  <si>
-    <t>Group ID</t>
   </si>
   <si>
     <t>data gap</t>
@@ -1012,6 +1006,12 @@
   </si>
   <si>
     <t>Unclassified</t>
+  </si>
+  <si>
+    <t>Ecosystem_functional_group</t>
+  </si>
+  <si>
+    <t>Group_ID</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1077,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1105,16 +1105,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1451,38 +1453,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F06308A-2E28-46FE-9E09-C3F62953F32E}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="51.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="9"/>
+    <col min="2" max="2" width="51.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" style="9" customWidth="1"/>
     <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.453125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1491,34 +1494,34 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>216</v>
+      <c r="H1" s="8" t="s">
+        <v>322</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="9" t="str">
         <f t="shared" ref="B2:B43" si="0">CONCATENATE(H2," ",G2)</f>
         <v>F1.1 Permanent upland streams</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
@@ -1527,34 +1530,34 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F1.2 Permanent lowland rivers</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
@@ -1563,34 +1566,34 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F1.3 Freeze-thaw rivers and streams</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
@@ -1599,34 +1602,34 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F1.4 Seasonal upland streams</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
@@ -1635,34 +1638,34 @@
       <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F1.5 Seasonal lowland rivers</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
@@ -1671,34 +1674,34 @@
       <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F1.6 Episodic arid rivers</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
@@ -1707,64 +1710,64 @@
       <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>269</v>
-      </c>
-      <c r="H8" t="s">
-        <v>270</v>
+        <v>267</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>268</v>
       </c>
       <c r="I8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.1 Large permanent freshwater lakes</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F9" t="s">
@@ -1773,34 +1776,34 @@
       <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.2 Small permanent freshwater lakes</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F10" t="s">
@@ -1809,34 +1812,34 @@
       <c r="G10" t="s">
         <v>26</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.3 Seasonal freshwater lakes</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F11" t="s">
@@ -1845,69 +1848,69 @@
       <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="9" t="s">
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>271</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F12" t="s">
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>272</v>
-      </c>
-      <c r="H12" t="s">
-        <v>273</v>
+        <v>270</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="I12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.5 Ephemeral freshwater lakes</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F13" t="s">
@@ -1916,34 +1919,34 @@
       <c r="G13" t="s">
         <v>30</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="9" t="s">
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.6 Permanent salt and soda lakes</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F14" t="s">
@@ -1952,34 +1955,34 @@
       <c r="G14" t="s">
         <v>32</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>240</v>
+      <c r="I14" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.7 Ephemeral salt lakes</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F15" t="s">
@@ -1988,34 +1991,34 @@
       <c r="G15" t="s">
         <v>34</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>240</v>
+      <c r="I15" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F2.8 Artesian springs and oases</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F16" t="s">
@@ -2024,94 +2027,94 @@
       <c r="G16" t="s">
         <v>36</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>274</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>278</v>
-      </c>
-      <c r="H17" t="s">
         <v>276</v>
       </c>
+      <c r="H17" s="9" t="s">
+        <v>274</v>
+      </c>
       <c r="I17" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>275</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>279</v>
-      </c>
-      <c r="H18" t="s">
         <v>277</v>
       </c>
+      <c r="H18" s="9" t="s">
+        <v>275</v>
+      </c>
       <c r="I18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F3.1 Large reservoirs</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F19" t="s">
@@ -2120,32 +2123,32 @@
       <c r="G19" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="9" t="s">
         <v>41</v>
       </c>
       <c r="I19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F3.2 Constructed lacustrine wetlands</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F20" t="s">
@@ -2154,32 +2157,32 @@
       <c r="G20" t="s">
         <v>42</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="9" t="s">
         <v>43</v>
       </c>
       <c r="I20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B21" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F3.3 Rice paddies</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F21" t="s">
@@ -2188,32 +2191,32 @@
       <c r="G21" t="s">
         <v>44</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B22" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F3.4 Freshwater aquafarms</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F22" t="s">
@@ -2222,32 +2225,32 @@
       <c r="G22" t="s">
         <v>46</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="9" t="s">
         <v>47</v>
       </c>
       <c r="I22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B23" s="9" t="str">
         <f t="shared" si="0"/>
         <v>F3.5 Canals, ditches and drains</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F23" t="s">
@@ -2256,62 +2259,62 @@
       <c r="G23" t="s">
         <v>48</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="9" t="s">
         <v>49</v>
       </c>
       <c r="I23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>259</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F24" t="s">
         <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>261</v>
-      </c>
-      <c r="H24" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="I24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B25" s="9" t="str">
         <f>CONCATENATE(H25," ",G25)</f>
         <v>FM1.2 Permanently open riverine estuaries and bays</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D25" t="s">
         <v>51</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F25" t="s">
@@ -2320,34 +2323,34 @@
       <c r="G25" t="s">
         <v>54</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="9" t="s">
         <v>55</v>
       </c>
       <c r="I25" t="s">
+        <v>212</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>214</v>
-      </c>
       <c r="K25" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B26" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FM1.3 Intermittently closed and open lakes and lagoons</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F26" t="s">
@@ -2356,64 +2359,64 @@
       <c r="G26" t="s">
         <v>56</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>264</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D27" t="s">
         <v>59</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="9" t="s">
         <v>60</v>
       </c>
       <c r="F27" t="s">
         <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>262</v>
-      </c>
-      <c r="H27" t="s">
-        <v>263</v>
+        <v>260</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>261</v>
       </c>
       <c r="I27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" t="str">
+      <c r="B28" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MFT1.2 Intertidal forests and shrublands</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D28" t="s">
         <v>59</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="9" t="s">
         <v>60</v>
       </c>
       <c r="F28" t="s">
@@ -2422,32 +2425,32 @@
       <c r="G28" t="s">
         <v>62</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>239</v>
+      <c r="I28" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="7" t="s">
-        <v>230</v>
+      <c r="K28" s="6" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" t="str">
+      <c r="B29" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MFT1.3 Coastal saltmarshes and reedbeds</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D29" t="s">
         <v>59</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="9" t="s">
         <v>60</v>
       </c>
       <c r="F29" t="s">
@@ -2456,32 +2459,32 @@
       <c r="G29" t="s">
         <v>64</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>239</v>
+      <c r="I29" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
-      <c r="B30" t="str">
+      <c r="B30" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MT1.1 Rocky Shorelines</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>67</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="9" t="s">
         <v>68</v>
       </c>
       <c r="F30" t="s">
@@ -2490,34 +2493,34 @@
       <c r="G30" t="s">
         <v>70</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="9" t="s">
         <v>71</v>
       </c>
       <c r="I30" t="s">
+        <v>232</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>236</v>
-      </c>
       <c r="K30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" t="str">
+      <c r="B31" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MT1.2 Muddy Shorelines</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D31" t="s">
         <v>67</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="9" t="s">
         <v>68</v>
       </c>
       <c r="F31" t="s">
@@ -2526,32 +2529,32 @@
       <c r="G31" t="s">
         <v>72</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="9" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" t="str">
+      <c r="B32" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MT1.3 Sandy Shorelines</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D32" t="s">
         <v>67</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="9" t="s">
         <v>68</v>
       </c>
       <c r="F32" t="s">
@@ -2560,34 +2563,34 @@
       <c r="G32" t="s">
         <v>74</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="9" t="s">
         <v>75</v>
       </c>
       <c r="I32" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B33" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MT1.4 Boulder and cobble shores</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>67</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="9" t="s">
         <v>68</v>
       </c>
       <c r="F33" t="s">
@@ -2596,31 +2599,31 @@
       <c r="G33" t="s">
         <v>76</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="9" t="s">
         <v>77</v>
       </c>
       <c r="I33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MT2.1 Coastal shrublands and grasslands</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D34" t="s">
         <v>67</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="9" t="s">
         <v>78</v>
       </c>
       <c r="F34" t="s">
@@ -2629,62 +2632,62 @@
       <c r="G34" t="s">
         <v>80</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="9" t="s">
         <v>81</v>
       </c>
       <c r="I34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D35" t="s">
         <v>67</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="9" t="s">
         <v>78</v>
       </c>
       <c r="F35" t="s">
         <v>79</v>
       </c>
       <c r="G35" t="s">
-        <v>258</v>
-      </c>
-      <c r="H35" t="s">
         <v>256</v>
       </c>
+      <c r="H35" s="9" t="s">
+        <v>254</v>
+      </c>
       <c r="I35" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36" s="9" t="str">
         <f t="shared" si="0"/>
         <v>MT3.1 Artificial shorelines</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D36" t="s">
         <v>67</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F36" t="s">
@@ -2693,31 +2696,31 @@
       <c r="G36" t="s">
         <v>84</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="9" t="s">
         <v>85</v>
       </c>
       <c r="I36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K36" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" t="str">
+      <c r="B37" s="9" t="str">
         <f t="shared" si="0"/>
         <v>T1.1 Tropical/Subtropical lowland rainforests</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D37" t="s">
         <v>87</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F37" t="s">
@@ -2726,31 +2729,31 @@
       <c r="G37" t="s">
         <v>90</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="9" t="s">
         <v>91</v>
       </c>
       <c r="I37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B38" s="9" t="str">
         <f t="shared" si="0"/>
         <v>T1.2 Tropical/Subtropical dry forests and thickets</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D38" t="s">
         <v>87</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F38" t="s">
@@ -2759,31 +2762,31 @@
       <c r="G38" t="s">
         <v>92</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="9" t="s">
         <v>93</v>
       </c>
       <c r="I38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" t="str">
+      <c r="B39" s="9" t="str">
         <f t="shared" si="0"/>
         <v>T1.3 Tropical/Subtropical montane rainforests</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D39" t="s">
         <v>87</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F39" t="s">
@@ -2792,118 +2795,118 @@
       <c r="G39" t="s">
         <v>94</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="9" t="s">
         <v>95</v>
       </c>
       <c r="I39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40">
+      <c r="A40" s="9">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>280</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D40" t="s">
         <v>87</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F40" t="s">
         <v>89</v>
       </c>
       <c r="G40" t="s">
+        <v>279</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I40" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" s="9">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="H40" t="s">
-        <v>282</v>
-      </c>
-      <c r="I40" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>283</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C41" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D41" t="s">
         <v>87</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F41" t="s">
         <v>97</v>
       </c>
       <c r="G41" t="s">
-        <v>287</v>
-      </c>
-      <c r="H41" t="s">
         <v>285</v>
       </c>
+      <c r="H41" s="9" t="s">
+        <v>283</v>
+      </c>
       <c r="I41" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
-        <v>284</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D42" t="s">
         <v>87</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F42" t="s">
         <v>97</v>
       </c>
       <c r="G42" t="s">
-        <v>288</v>
-      </c>
-      <c r="H42" t="s">
         <v>286</v>
       </c>
+      <c r="H42" s="9" t="s">
+        <v>284</v>
+      </c>
       <c r="I42" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B43" s="9" t="str">
         <f t="shared" si="0"/>
         <v>T2.3 Oceanic cool temperate rainforests</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D43" t="s">
         <v>87</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F43" t="s">
@@ -2912,31 +2915,31 @@
       <c r="G43" t="s">
         <v>98</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="9" t="s">
         <v>99</v>
       </c>
       <c r="I43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K43" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
-      <c r="B44" t="str">
+      <c r="B44" s="9" t="str">
         <f t="shared" ref="B44:B85" si="1">CONCATENATE(H44," ",G44)</f>
         <v>T2.4 Warm temperate laurophyll forests</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D44" t="s">
         <v>87</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F44" t="s">
@@ -2945,31 +2948,31 @@
       <c r="G44" t="s">
         <v>100</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I44" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B45" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T2.5 Temperate pyric humid forests</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D45" t="s">
         <v>87</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F45" t="s">
@@ -2978,31 +2981,31 @@
       <c r="G45" t="s">
         <v>102</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="9" t="s">
         <v>103</v>
       </c>
       <c r="I45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
-      <c r="B46" t="str">
+      <c r="B46" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T2.6 Temperate pyric sclerophyll forests and woodlands</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D46" t="s">
         <v>87</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F46" t="s">
@@ -3011,31 +3014,31 @@
       <c r="G46" t="s">
         <v>104</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="9" t="s">
         <v>105</v>
       </c>
       <c r="I46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K46" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47">
+      <c r="A47" s="9">
         <v>46</v>
       </c>
-      <c r="B47" t="str">
+      <c r="B47" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T3.1 Seasonally dry tropical shrublands</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D47" t="s">
         <v>87</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F47" t="s">
@@ -3044,31 +3047,31 @@
       <c r="G47" t="s">
         <v>108</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="9" t="s">
         <v>109</v>
       </c>
       <c r="I47" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K47" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48">
+      <c r="A48" s="9">
         <v>47</v>
       </c>
-      <c r="B48" t="str">
+      <c r="B48" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T3.2 Seasonally dry temperate heath and shrublands</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D48" t="s">
         <v>87</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F48" t="s">
@@ -3077,118 +3080,118 @@
       <c r="G48" t="s">
         <v>110</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="9" t="s">
         <v>111</v>
       </c>
       <c r="I48" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K48" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49">
+      <c r="A49" s="9">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>289</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D49" t="s">
         <v>87</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F49" t="s">
         <v>107</v>
       </c>
       <c r="G49" t="s">
-        <v>293</v>
-      </c>
-      <c r="H49" t="s">
         <v>291</v>
       </c>
+      <c r="H49" s="9" t="s">
+        <v>289</v>
+      </c>
       <c r="I49" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50">
+      <c r="A50" s="9">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>290</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B50" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>87</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F50" t="s">
         <v>107</v>
       </c>
       <c r="G50" t="s">
-        <v>294</v>
-      </c>
-      <c r="H50" t="s">
         <v>292</v>
       </c>
+      <c r="H50" s="9" t="s">
+        <v>290</v>
+      </c>
       <c r="I50" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51">
+      <c r="A51" s="9">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
-        <v>295</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D51" t="s">
         <v>87</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F51" t="s">
         <v>113</v>
       </c>
       <c r="G51" t="s">
-        <v>296</v>
-      </c>
-      <c r="H51" t="s">
-        <v>297</v>
+        <v>294</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>295</v>
       </c>
       <c r="I51" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52">
+      <c r="A52" s="9">
         <v>51</v>
       </c>
-      <c r="B52" t="str">
+      <c r="B52" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T4.2 Pyric tussock savannas</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D52" t="s">
         <v>87</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F52" t="s">
@@ -3197,31 +3200,31 @@
       <c r="G52" t="s">
         <v>114</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="9" t="s">
         <v>115</v>
       </c>
       <c r="I52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K52" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53">
+      <c r="A53" s="9">
         <v>52</v>
       </c>
-      <c r="B53" t="str">
+      <c r="B53" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T4.3 Hummock savannas</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D53" t="s">
         <v>87</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F53" t="s">
@@ -3230,31 +3233,31 @@
       <c r="G53" t="s">
         <v>116</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="9" t="s">
         <v>117</v>
       </c>
       <c r="I53" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K53" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54">
+      <c r="A54" s="9">
         <v>53</v>
       </c>
-      <c r="B54" t="str">
+      <c r="B54" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T4.4 Temperate woodlands</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D54" t="s">
         <v>87</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F54" t="s">
@@ -3263,31 +3266,31 @@
       <c r="G54" t="s">
         <v>118</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="9" t="s">
         <v>119</v>
       </c>
       <c r="I54" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K54" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55">
+      <c r="A55" s="9">
         <v>54</v>
       </c>
-      <c r="B55" t="str">
+      <c r="B55" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T4.5 Temperate subhumid grasslands</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D55" t="s">
         <v>87</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F55" t="s">
@@ -3296,31 +3299,31 @@
       <c r="G55" t="s">
         <v>120</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="9" t="s">
         <v>121</v>
       </c>
       <c r="I55" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K55" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56">
+      <c r="A56" s="9">
         <v>55</v>
       </c>
-      <c r="B56" t="str">
+      <c r="B56" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T5.1 Semi-desert steppe</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D56" t="s">
         <v>87</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="9" t="s">
         <v>122</v>
       </c>
       <c r="F56" t="s">
@@ -3329,60 +3332,60 @@
       <c r="G56" t="s">
         <v>124</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="9" t="s">
         <v>125</v>
       </c>
       <c r="I56" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K56" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57">
+      <c r="A57" s="9">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>298</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B57" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D57" t="s">
         <v>87</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="9" t="s">
         <v>122</v>
       </c>
       <c r="F57" t="s">
         <v>123</v>
       </c>
       <c r="G57" t="s">
-        <v>308</v>
-      </c>
-      <c r="H57" t="s">
-        <v>303</v>
+        <v>306</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="I57" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A58">
+      <c r="A58" s="9">
         <v>57</v>
       </c>
-      <c r="B58" t="str">
+      <c r="B58" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T5.3 Sclerophyll hot deserts and semi-deserts</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D58" t="s">
         <v>87</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="9" t="s">
         <v>122</v>
       </c>
       <c r="F58" t="s">
@@ -3391,147 +3394,147 @@
       <c r="G58" t="s">
         <v>126</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="9" t="s">
         <v>127</v>
       </c>
       <c r="I58" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A59">
+      <c r="A59" s="9">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
-        <v>299</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B59" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D59" t="s">
         <v>87</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="9" t="s">
         <v>122</v>
       </c>
       <c r="F59" t="s">
         <v>123</v>
       </c>
       <c r="G59" t="s">
-        <v>309</v>
-      </c>
-      <c r="H59" t="s">
-        <v>304</v>
+        <v>307</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>302</v>
       </c>
       <c r="I59" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A60">
+      <c r="A60" s="9">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>300</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B60" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="9" t="s">
         <v>122</v>
       </c>
       <c r="F60" t="s">
         <v>123</v>
       </c>
       <c r="G60" t="s">
-        <v>310</v>
-      </c>
-      <c r="H60" t="s">
-        <v>305</v>
+        <v>308</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="I60" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61">
+      <c r="A61" s="9">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
-        <v>301</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B61" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D61" t="s">
         <v>87</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F61" t="s">
         <v>129</v>
       </c>
       <c r="G61" t="s">
-        <v>311</v>
-      </c>
-      <c r="H61" t="s">
-        <v>306</v>
+        <v>309</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>304</v>
       </c>
       <c r="I61" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62">
+      <c r="A62" s="9">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
-        <v>302</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B62" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D62" t="s">
         <v>87</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F62" t="s">
         <v>129</v>
       </c>
       <c r="G62" t="s">
-        <v>312</v>
-      </c>
-      <c r="H62" t="s">
-        <v>307</v>
+        <v>310</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>305</v>
       </c>
       <c r="I62" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A63">
+      <c r="A63" s="9">
         <v>62</v>
       </c>
-      <c r="B63" t="str">
+      <c r="B63" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T6.3 Polar tundra and deserts</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D63" t="s">
         <v>87</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F63" t="s">
@@ -3540,31 +3543,31 @@
       <c r="G63" t="s">
         <v>130</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="9" t="s">
         <v>131</v>
       </c>
       <c r="I63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K63" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64">
+      <c r="A64" s="9">
         <v>63</v>
       </c>
-      <c r="B64" t="str">
+      <c r="B64" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T6.4 Temperate alpine grasslands and shrublands</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D64" t="s">
         <v>87</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F64" t="s">
@@ -3573,60 +3576,60 @@
       <c r="G64" t="s">
         <v>132</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="9" t="s">
         <v>133</v>
       </c>
       <c r="I64" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65">
+      <c r="A65" s="9">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>313</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B65" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D65" t="s">
         <v>87</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F65" t="s">
         <v>129</v>
       </c>
       <c r="G65" t="s">
-        <v>314</v>
-      </c>
-      <c r="H65" t="s">
-        <v>315</v>
+        <v>312</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>313</v>
       </c>
       <c r="I65" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66">
+      <c r="A66" s="9">
         <v>65</v>
       </c>
-      <c r="B66" t="str">
+      <c r="B66" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T7.1 Annual croplands</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D66" t="s">
         <v>87</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="9" t="s">
         <v>134</v>
       </c>
       <c r="F66" t="s">
@@ -3635,31 +3638,31 @@
       <c r="G66" t="s">
         <v>136</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="9" t="s">
         <v>137</v>
       </c>
       <c r="I66" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K66" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67">
+      <c r="A67" s="9">
         <v>66</v>
       </c>
-      <c r="B67" t="str">
+      <c r="B67" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T7.2 Sown pastures and fields</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D67" t="s">
         <v>87</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="9" t="s">
         <v>134</v>
       </c>
       <c r="F67" t="s">
@@ -3668,31 +3671,31 @@
       <c r="G67" t="s">
         <v>138</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="9" t="s">
         <v>139</v>
       </c>
       <c r="I67" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K67" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68">
+      <c r="A68" s="9">
         <v>67</v>
       </c>
-      <c r="B68" t="str">
+      <c r="B68" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T7.3 Plantations</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D68" t="s">
         <v>87</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="9" t="s">
         <v>134</v>
       </c>
       <c r="F68" t="s">
@@ -3701,31 +3704,31 @@
       <c r="G68" t="s">
         <v>140</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I68" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K68" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69">
+      <c r="A69" s="9">
         <v>68</v>
       </c>
-      <c r="B69" t="str">
+      <c r="B69" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T7.4 Urban and industrial ecosystems</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D69" t="s">
         <v>87</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="9" t="s">
         <v>134</v>
       </c>
       <c r="F69" t="s">
@@ -3734,31 +3737,31 @@
       <c r="G69" t="s">
         <v>142</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="9" t="s">
         <v>143</v>
       </c>
       <c r="I69" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70">
+      <c r="A70" s="9">
         <v>69</v>
       </c>
-      <c r="B70" t="str">
+      <c r="B70" s="9" t="str">
         <f t="shared" si="1"/>
         <v>T7.5 Derived semi-natural pastures and old fields</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D70" t="s">
         <v>87</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="9" t="s">
         <v>134</v>
       </c>
       <c r="F70" t="s">
@@ -3767,60 +3770,60 @@
       <c r="G70" t="s">
         <v>144</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="9" t="s">
         <v>145</v>
       </c>
       <c r="I70" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K70" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71">
+      <c r="A71" s="9">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
-        <v>316</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B71" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D71" t="s">
         <v>147</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F71" t="s">
         <v>149</v>
       </c>
       <c r="G71" t="s">
-        <v>317</v>
-      </c>
-      <c r="H71" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="I71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72">
+      <c r="A72" s="9">
         <v>71</v>
       </c>
-      <c r="B72" t="str">
+      <c r="B72" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TF1.2 Subtropical/temperate forested wetlands</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D72" t="s">
         <v>147</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F72" t="s">
@@ -3829,31 +3832,31 @@
       <c r="G72" t="s">
         <v>150</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="9" t="s">
         <v>151</v>
       </c>
       <c r="I72" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73">
+      <c r="A73" s="9">
         <v>72</v>
       </c>
-      <c r="B73" t="str">
+      <c r="B73" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TF1.3 Permanent marshes</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D73" t="s">
         <v>147</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F73" t="s">
@@ -3862,31 +3865,31 @@
       <c r="G73" t="s">
         <v>152</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73" s="9" t="s">
         <v>153</v>
       </c>
       <c r="I73" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K73" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74">
+      <c r="A74" s="9">
         <v>73</v>
       </c>
-      <c r="B74" t="str">
+      <c r="B74" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TF1.4 Seasonal floodplain marshes</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D74" t="s">
         <v>147</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F74" t="s">
@@ -3895,31 +3898,31 @@
       <c r="G74" t="s">
         <v>154</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H74" s="9" t="s">
         <v>155</v>
       </c>
       <c r="I74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K74" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75">
+      <c r="A75" s="9">
         <v>74</v>
       </c>
-      <c r="B75" t="str">
+      <c r="B75" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TF1.5 Episodic arid floodplains</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D75" t="s">
         <v>147</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F75" t="s">
@@ -3928,31 +3931,31 @@
       <c r="G75" t="s">
         <v>156</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H75" s="9" t="s">
         <v>157</v>
       </c>
       <c r="I75" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K75" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76">
+      <c r="A76" s="9">
         <v>75</v>
       </c>
-      <c r="B76" t="str">
+      <c r="B76" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TF1.6 Boreal, temperate and montane peat bogs</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D76" t="s">
         <v>147</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F76" t="s">
@@ -3961,60 +3964,60 @@
       <c r="G76" t="s">
         <v>158</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="9" t="s">
         <v>159</v>
       </c>
       <c r="I76" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K76" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77">
+      <c r="A77" s="9">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
-        <v>265</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B77" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D77" t="s">
         <v>147</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="9" t="s">
         <v>148</v>
       </c>
       <c r="F77" t="s">
         <v>149</v>
       </c>
       <c r="G77" t="s">
-        <v>267</v>
-      </c>
-      <c r="H77" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="I77" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A78">
+      <c r="A78" s="9">
         <v>77</v>
       </c>
-      <c r="B78" t="str">
+      <c r="B78" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.1 Seagrass meadows</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D78" t="s">
         <v>161</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F78" t="s">
@@ -4023,32 +4026,32 @@
       <c r="G78" t="s">
         <v>164</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H78" s="9" t="s">
         <v>165</v>
       </c>
       <c r="I78" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J78" s="2"/>
-      <c r="K78" s="7" t="s">
-        <v>228</v>
+      <c r="K78" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79">
+      <c r="A79" s="9">
         <v>79</v>
       </c>
-      <c r="B79" t="str">
+      <c r="B79" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.2 Kelp forests</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D79" t="s">
         <v>161</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F79" t="s">
@@ -4057,31 +4060,31 @@
       <c r="G79" t="s">
         <v>168</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="9" t="s">
         <v>169</v>
       </c>
       <c r="I79" t="s">
+        <v>215</v>
+      </c>
+      <c r="J79" t="s">
         <v>217</v>
       </c>
-      <c r="J79" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80">
+      <c r="A80" s="9">
         <v>80</v>
       </c>
-      <c r="B80" t="str">
+      <c r="B80" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.3 Photic coral reefs</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D80" t="s">
         <v>161</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F80" t="s">
@@ -4090,31 +4093,31 @@
       <c r="G80" t="s">
         <v>170</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="9" t="s">
         <v>171</v>
       </c>
       <c r="I80" t="s">
-        <v>232</v>
-      </c>
-      <c r="K80" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81">
+      <c r="A81" s="9">
         <v>81</v>
       </c>
-      <c r="B81" t="str">
+      <c r="B81" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.4 Shellfish beds and reefs</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D81" t="s">
         <v>161</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F81" t="s">
@@ -4123,31 +4126,31 @@
       <c r="G81" t="s">
         <v>172</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="9" t="s">
         <v>173</v>
       </c>
       <c r="I81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J81" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82">
+      <c r="A82" s="9">
         <v>82</v>
       </c>
-      <c r="B82" t="str">
+      <c r="B82" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.5 Photo-limited marine animal forests</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D82" t="s">
         <v>161</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F82" t="s">
@@ -4156,31 +4159,31 @@
       <c r="G82" t="s">
         <v>174</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H82" s="9" t="s">
         <v>175</v>
       </c>
       <c r="I82" t="s">
-        <v>232</v>
-      </c>
-      <c r="K82" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83">
+      <c r="A83" s="9">
         <v>83</v>
       </c>
-      <c r="B83" t="str">
+      <c r="B83" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.6 Subtidal rocky reefs</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D83" t="s">
         <v>161</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F83" t="s">
@@ -4189,31 +4192,31 @@
       <c r="G83" t="s">
         <v>176</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="9" t="s">
         <v>177</v>
       </c>
       <c r="I83" t="s">
-        <v>232</v>
-      </c>
-      <c r="K83" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84">
+      <c r="A84" s="9">
         <v>84</v>
       </c>
-      <c r="B84" t="str">
+      <c r="B84" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.7 Subtidal sand beds</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D84" t="s">
         <v>161</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F84" t="s">
@@ -4222,31 +4225,31 @@
       <c r="G84" t="s">
         <v>178</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="9" t="s">
         <v>179</v>
       </c>
       <c r="I84" t="s">
-        <v>232</v>
-      </c>
-      <c r="K84" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85">
+      <c r="A85" s="9">
         <v>85</v>
       </c>
-      <c r="B85" t="str">
+      <c r="B85" s="9" t="str">
         <f t="shared" si="1"/>
         <v>M1.8 Subtidal mud plains</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D85" t="s">
         <v>161</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F85" t="s">
@@ -4255,61 +4258,61 @@
       <c r="G85" t="s">
         <v>180</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H85" s="9" t="s">
         <v>181</v>
       </c>
       <c r="I85" t="s">
-        <v>232</v>
-      </c>
-      <c r="K85" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A86">
+      <c r="A86" s="9">
         <v>86</v>
       </c>
-      <c r="B86" t="s">
-        <v>243</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B86" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D86" t="s">
         <v>161</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F86" t="s">
         <v>163</v>
       </c>
       <c r="G86" t="s">
+        <v>242</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="I86" t="s">
         <v>244</v>
       </c>
-      <c r="H86" t="s">
-        <v>245</v>
-      </c>
-      <c r="I86" t="s">
-        <v>246</v>
-      </c>
-      <c r="K86" s="7"/>
+      <c r="K86" s="6"/>
     </row>
     <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87">
+      <c r="A87" s="9">
         <v>78</v>
       </c>
-      <c r="B87" t="str">
+      <c r="B87" s="9" t="str">
         <f>CONCATENATE(H87," ",G87)</f>
         <v>M1.10 Rhodolith/Maërl beds</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D87" t="s">
         <v>161</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F87" t="s">
@@ -4318,31 +4321,31 @@
       <c r="G87" t="s">
         <v>166</v>
       </c>
-      <c r="H87" t="s">
+      <c r="H87" s="9" t="s">
         <v>167</v>
       </c>
       <c r="I87" t="s">
-        <v>232</v>
-      </c>
-      <c r="K87" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88">
+      <c r="A88" s="9">
         <v>87</v>
       </c>
-      <c r="B88" t="str">
+      <c r="B88" s="9" t="str">
         <f t="shared" ref="B88:B102" si="2">CONCATENATE(H88," ",G88)</f>
         <v>M2.1 Epipelagic ocean waters</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D88" t="s">
         <v>161</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="9" t="s">
         <v>182</v>
       </c>
       <c r="F88" t="s">
@@ -4351,31 +4354,31 @@
       <c r="G88" t="s">
         <v>184</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H88" s="9" t="s">
         <v>185</v>
       </c>
       <c r="I88" t="s">
-        <v>231</v>
-      </c>
-      <c r="K88" s="7" t="s">
         <v>229</v>
       </c>
+      <c r="K88" s="6" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A89">
+      <c r="A89" s="9">
         <v>88</v>
       </c>
-      <c r="B89" t="str">
+      <c r="B89" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M2.2 Mesopelagic ocean water</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D89" t="s">
         <v>161</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="9" t="s">
         <v>182</v>
       </c>
       <c r="F89" t="s">
@@ -4384,31 +4387,31 @@
       <c r="G89" t="s">
         <v>186</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="9" t="s">
         <v>187</v>
       </c>
       <c r="I89" t="s">
-        <v>231</v>
-      </c>
-      <c r="K89" s="7" t="s">
         <v>229</v>
       </c>
+      <c r="K89" s="6" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A90">
+      <c r="A90" s="9">
         <v>89</v>
       </c>
-      <c r="B90" t="str">
+      <c r="B90" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M2.3 Bathypelagic ocean waters</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D90" t="s">
         <v>161</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="9" t="s">
         <v>182</v>
       </c>
       <c r="F90" t="s">
@@ -4417,31 +4420,31 @@
       <c r="G90" t="s">
         <v>188</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="9" t="s">
         <v>189</v>
       </c>
       <c r="I90" t="s">
-        <v>231</v>
-      </c>
-      <c r="K90" s="7" t="s">
         <v>229</v>
       </c>
+      <c r="K90" s="6" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A91">
+      <c r="A91" s="9">
         <v>90</v>
       </c>
-      <c r="B91" t="str">
+      <c r="B91" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M2.4 Abyssopelagic ocean waters</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D91" t="s">
         <v>161</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="9" t="s">
         <v>182</v>
       </c>
       <c r="F91" t="s">
@@ -4450,30 +4453,30 @@
       <c r="G91" t="s">
         <v>190</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="9" t="s">
         <v>191</v>
       </c>
       <c r="I91" t="s">
-        <v>231</v>
-      </c>
-      <c r="K91" s="7" t="s">
         <v>229</v>
       </c>
+      <c r="K91" s="6" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A92">
+      <c r="A92" s="9">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
-        <v>247</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B92" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D92" t="s">
         <v>161</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="9" t="s">
         <v>182</v>
       </c>
       <c r="F92" t="s">
@@ -4482,29 +4485,29 @@
       <c r="G92" t="s">
         <v>190</v>
       </c>
-      <c r="H92" t="s">
-        <v>249</v>
+      <c r="H92" s="9" t="s">
+        <v>247</v>
       </c>
       <c r="I92" t="s">
-        <v>248</v>
-      </c>
-      <c r="K92" s="7"/>
+        <v>246</v>
+      </c>
+      <c r="K92" s="6"/>
     </row>
     <row r="93" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A93">
+      <c r="A93" s="9">
         <v>92</v>
       </c>
-      <c r="B93" t="str">
+      <c r="B93" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M3.1 Continental and island slopes</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D93" t="s">
         <v>161</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F93" t="s">
@@ -4513,31 +4516,31 @@
       <c r="G93" t="s">
         <v>194</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93" s="9" t="s">
         <v>195</v>
       </c>
       <c r="I93" t="s">
-        <v>232</v>
-      </c>
-      <c r="K93" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A94">
+      <c r="A94" s="9">
         <v>93</v>
       </c>
-      <c r="B94" t="str">
+      <c r="B94" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M3.2 Submarine canyons</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D94" t="s">
         <v>161</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F94" t="s">
@@ -4546,31 +4549,31 @@
       <c r="G94" t="s">
         <v>196</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H94" s="9" t="s">
         <v>197</v>
       </c>
       <c r="I94" t="s">
-        <v>232</v>
-      </c>
-      <c r="K94" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K94" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A95">
+      <c r="A95" s="9">
         <v>94</v>
       </c>
-      <c r="B95" t="str">
+      <c r="B95" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M3.3 Abyssal plains</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D95" t="s">
         <v>161</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F95" t="s">
@@ -4579,31 +4582,31 @@
       <c r="G95" t="s">
         <v>198</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H95" s="9" t="s">
         <v>199</v>
       </c>
       <c r="I95" t="s">
-        <v>232</v>
-      </c>
-      <c r="K95" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A96">
+      <c r="A96" s="9">
         <v>95</v>
       </c>
-      <c r="B96" t="str">
+      <c r="B96" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M3.4 Seamounts, ridges and plateaus</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D96" t="s">
         <v>161</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F96" t="s">
@@ -4612,30 +4615,30 @@
       <c r="G96" t="s">
         <v>200</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H96" s="9" t="s">
         <v>201</v>
       </c>
       <c r="I96" t="s">
-        <v>232</v>
-      </c>
-      <c r="K96" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="K96" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A97">
+      <c r="A97" s="9">
         <v>96</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="B97" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C97" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D97" t="s">
         <v>161</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F97" t="s">
@@ -4644,28 +4647,28 @@
       <c r="G97" t="s">
         <v>200</v>
       </c>
-      <c r="H97" t="s">
-        <v>253</v>
+      <c r="H97" s="9" t="s">
+        <v>251</v>
       </c>
       <c r="I97" t="s">
-        <v>217</v>
-      </c>
-      <c r="K97" s="7"/>
+        <v>215</v>
+      </c>
+      <c r="K97" s="6"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A98">
+      <c r="A98" s="9">
         <v>97</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B98" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D98" t="s">
         <v>161</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F98" t="s">
@@ -4674,28 +4677,28 @@
       <c r="G98" t="s">
         <v>200</v>
       </c>
-      <c r="H98" t="s">
-        <v>254</v>
+      <c r="H98" s="9" t="s">
+        <v>252</v>
       </c>
       <c r="I98" t="s">
-        <v>217</v>
-      </c>
-      <c r="K98" s="7"/>
+        <v>215</v>
+      </c>
+      <c r="K98" s="6"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A99">
+      <c r="A99" s="9">
         <v>98</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B99" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D99" t="s">
         <v>161</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F99" t="s">
@@ -4704,29 +4707,29 @@
       <c r="G99" t="s">
         <v>200</v>
       </c>
-      <c r="H99" t="s">
-        <v>255</v>
+      <c r="H99" s="9" t="s">
+        <v>253</v>
       </c>
       <c r="I99" t="s">
-        <v>217</v>
-      </c>
-      <c r="K99" s="7"/>
+        <v>215</v>
+      </c>
+      <c r="K99" s="6"/>
     </row>
     <row r="100" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A100">
+      <c r="A100" s="9">
         <v>99</v>
       </c>
-      <c r="B100" t="str">
+      <c r="B100" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M4.1 Submerged artificial structures</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D100" t="s">
         <v>161</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="9" t="s">
         <v>202</v>
       </c>
       <c r="F100" t="s">
@@ -4735,7 +4738,7 @@
       <c r="G100" t="s">
         <v>204</v>
       </c>
-      <c r="H100" t="s">
+      <c r="H100" s="9" t="s">
         <v>205</v>
       </c>
       <c r="I100" t="s">
@@ -4744,25 +4747,25 @@
       <c r="J100" t="s">
         <v>209</v>
       </c>
-      <c r="K100" s="7" t="s">
-        <v>229</v>
+      <c r="K100" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A101">
+      <c r="A101" s="9">
         <v>100</v>
       </c>
-      <c r="B101" t="str">
+      <c r="B101" s="9" t="str">
         <f t="shared" si="2"/>
         <v>M4.2 Marine aquafarms</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="9" t="s">
         <v>160</v>
       </c>
       <c r="D101" t="s">
         <v>161</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="9" t="s">
         <v>202</v>
       </c>
       <c r="F101" t="s">
@@ -4771,7 +4774,7 @@
       <c r="G101" t="s">
         <v>206</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H101" s="9" t="s">
         <v>207</v>
       </c>
       <c r="I101" t="s">
@@ -4780,56 +4783,62 @@
       <c r="J101" t="s">
         <v>210</v>
       </c>
-      <c r="K101" s="7" t="s">
-        <v>229</v>
+      <c r="K101" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A102">
+      <c r="A102" s="9">
         <v>101</v>
       </c>
-      <c r="B102" t="str">
+      <c r="B102" s="9" t="str">
         <f t="shared" si="2"/>
         <v>T4.4a Semi-arid woodlands</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D102" t="s">
         <v>87</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F102" t="s">
         <v>113</v>
       </c>
-      <c r="G102" s="9" t="s">
+      <c r="G102" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="H102" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="I102" t="s">
+        <v>239</v>
+      </c>
+      <c r="J102" t="s">
         <v>319</v>
       </c>
-      <c r="H102" t="s">
-        <v>320</v>
-      </c>
-      <c r="I102" t="s">
-        <v>241</v>
-      </c>
-      <c r="J102" t="s">
-        <v>321</v>
-      </c>
       <c r="K102" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A103">
+      <c r="A103" s="9">
         <v>255</v>
       </c>
-      <c r="B103" t="str">
+      <c r="B103" s="9" t="str">
         <f t="shared" ref="B103" si="3">CONCATENATE(H103," ",G103)</f>
         <v xml:space="preserve"> Unclassified</v>
       </c>
-      <c r="G103" s="9" t="s">
-        <v>322</v>
+      <c r="C103" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -5077,15 +5086,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="44e1a4a7-75d8-43f0-81dc-4aceded6063f">
@@ -5114,6 +5114,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99AD8296-EEAC-435D-8285-7496ACD2EECA}">
   <ds:schemaRefs>
@@ -5134,14 +5143,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E49A9ABC-A427-42A2-8F7A-D6C6654B9600}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36EA50D7-0A13-4ECA-8436-D4585B901078}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -5156,4 +5157,12 @@
     <ds:schemaRef ds:uri="27145d01-5063-4320-a0f8-74c9d44fede6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E49A9ABC-A427-42A2-8F7A-D6C6654B9600}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>